<commit_message>
Fix core form extension service bad mapping
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/extension-forms/xls/household_ext.xlsx
+++ b/src/main/resources/samples/extension-forms/xls/household_ext.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>type</t>
   </si>
@@ -112,15 +112,6 @@
   </si>
   <si>
     <t>Id do Formulário Mãe</t>
-  </si>
-  <si>
-    <t>visit_code</t>
-  </si>
-  <si>
-    <t>Visit Code</t>
-  </si>
-  <si>
-    <t>Código da Visita</t>
   </si>
   <si>
     <t>household_code</t>
@@ -353,8 +344,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -401,6 +392,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -408,18 +407,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -438,8 +438,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,14 +451,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -485,17 +478,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -509,29 +523,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -539,7 +530,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -578,7 +569,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,7 +629,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,7 +659,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,121 +683,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,6 +702,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,6 +757,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -786,6 +792,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -825,36 +846,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -867,159 +858,159 @@
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1107,9 +1098,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1487,14 +1475,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1546,7 +1534,7 @@
       <c r="I1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="28" t="s">
@@ -1558,7 +1546,7 @@
       <c r="M1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="34" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="28" t="s">
@@ -1601,24 +1589,24 @@
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="36" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
     </row>
     <row r="3" s="25" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
       <c r="A3" s="30" t="s">
@@ -1635,24 +1623,24 @@
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="36" t="s">
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
     </row>
     <row r="4" s="25" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
       <c r="A4" s="30" t="s">
@@ -1669,24 +1657,24 @@
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="36" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
     </row>
     <row r="5" s="26" customFormat="1" spans="1:14">
       <c r="A5" s="26" t="s">
@@ -1701,10 +1689,10 @@
       <c r="D5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1715,16 +1703,16 @@
       <c r="B6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1741,10 +1729,10 @@
       <c r="D7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1761,10 +1749,8 @@
       <c r="D8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" s="37" t="s">
+      <c r="J8" s="36"/>
+      <c r="N8" s="36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1781,250 +1767,228 @@
       <c r="D9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="36"/>
+      <c r="N9" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" s="26" customFormat="1" spans="1:14">
-      <c r="A10" s="26" t="s">
+    </row>
+    <row r="10" s="27" customFormat="1" spans="1:14">
+      <c r="A10" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="N10" s="37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" s="27" customFormat="1" spans="1:14">
+      <c r="D10" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="37"/>
+      <c r="N10" s="37"/>
+    </row>
+    <row r="11" s="27" customFormat="1" customHeight="1" spans="1:14">
       <c r="A11" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>47</v>
-      </c>
       <c r="D11" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="38"/>
-      <c r="N11" s="38"/>
-    </row>
-    <row r="12" s="27" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A12" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="38"/>
-      <c r="N12" s="38"/>
+        <v>46</v>
+      </c>
+      <c r="J11" s="37"/>
+      <c r="N11" s="37"/>
+    </row>
+    <row r="12" s="26" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J12" s="36"/>
+      <c r="N12" s="36"/>
     </row>
     <row r="13" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J13" s="37"/>
-      <c r="N13" s="37"/>
+      <c r="J13" s="36"/>
+      <c r="N13" s="36"/>
     </row>
     <row r="14" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J14" s="37"/>
-      <c r="N14" s="37"/>
+      <c r="J14" s="36"/>
+      <c r="N14" s="36"/>
     </row>
     <row r="15" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J15" s="37"/>
-      <c r="N15" s="37"/>
-    </row>
-    <row r="16" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J16" s="37"/>
-      <c r="N16" s="37"/>
-    </row>
-    <row r="17" s="26" customFormat="1" spans="10:14">
-      <c r="J17" s="37"/>
-      <c r="N17" s="37"/>
+      <c r="J15" s="36"/>
+      <c r="N15" s="36"/>
+    </row>
+    <row r="16" s="26" customFormat="1" spans="10:14">
+      <c r="J16" s="36"/>
+      <c r="N16" s="36"/>
+    </row>
+    <row r="17" s="26" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J17" s="36"/>
+      <c r="N17" s="36"/>
     </row>
     <row r="18" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J18" s="37"/>
-      <c r="N18" s="37"/>
+      <c r="J18" s="36"/>
+      <c r="N18" s="36"/>
     </row>
     <row r="19" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J19" s="37"/>
-      <c r="N19" s="37"/>
-    </row>
-    <row r="20" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="J19" s="36"/>
+      <c r="N19" s="36"/>
+    </row>
+    <row r="20" s="26" customFormat="1" spans="10:14">
+      <c r="J20" s="36"/>
+      <c r="N20" s="36"/>
     </row>
     <row r="21" s="26" customFormat="1" spans="10:14">
-      <c r="J21" s="37"/>
-      <c r="N21" s="37"/>
+      <c r="J21" s="36"/>
+      <c r="N21" s="36"/>
     </row>
     <row r="22" s="26" customFormat="1" spans="10:14">
-      <c r="J22" s="37"/>
-      <c r="N22" s="37"/>
-    </row>
-    <row r="23" s="26" customFormat="1" spans="10:14">
-      <c r="J23" s="37"/>
-      <c r="N23" s="37"/>
-    </row>
-    <row r="24" s="26" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
-      <c r="J24" s="37"/>
-      <c r="N24" s="37"/>
-    </row>
-    <row r="25" s="26" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J25" s="37"/>
-      <c r="N25" s="37"/>
+      <c r="J22" s="36"/>
+      <c r="N22" s="36"/>
+    </row>
+    <row r="23" s="26" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
+      <c r="J23" s="36"/>
+      <c r="N23" s="36"/>
+    </row>
+    <row r="24" s="26" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J24" s="36"/>
+      <c r="N24" s="36"/>
+    </row>
+    <row r="25" s="26" customFormat="1" spans="10:14">
+      <c r="J25" s="36"/>
+      <c r="N25" s="36"/>
     </row>
     <row r="26" s="26" customFormat="1" spans="10:14">
-      <c r="J26" s="37"/>
-      <c r="N26" s="37"/>
+      <c r="J26" s="36"/>
+      <c r="N26" s="36"/>
     </row>
     <row r="27" s="26" customFormat="1" spans="10:14">
-      <c r="J27" s="37"/>
-      <c r="N27" s="37"/>
-    </row>
-    <row r="28" s="26" customFormat="1" spans="10:14">
-      <c r="J28" s="37"/>
-      <c r="N28" s="37"/>
-    </row>
-    <row r="29" s="26" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J29" s="37"/>
-      <c r="N29" s="37"/>
+      <c r="J27" s="36"/>
+      <c r="N27" s="36"/>
+    </row>
+    <row r="28" s="26" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J28" s="36"/>
+      <c r="N28" s="36"/>
+    </row>
+    <row r="29" s="26" customFormat="1" spans="10:14">
+      <c r="J29" s="36"/>
+      <c r="N29" s="36"/>
     </row>
     <row r="30" s="26" customFormat="1" spans="10:14">
-      <c r="J30" s="37"/>
-      <c r="N30" s="37"/>
+      <c r="J30" s="36"/>
+      <c r="N30" s="36"/>
     </row>
     <row r="31" s="26" customFormat="1" spans="10:14">
-      <c r="J31" s="37"/>
-      <c r="N31" s="37"/>
+      <c r="J31" s="36"/>
+      <c r="N31" s="36"/>
     </row>
     <row r="32" s="26" customFormat="1" spans="10:14">
-      <c r="J32" s="37"/>
-      <c r="N32" s="37"/>
-    </row>
-    <row r="33" s="26" customFormat="1" spans="10:14">
-      <c r="J33" s="37"/>
-      <c r="N33" s="37"/>
-    </row>
-    <row r="34" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J34" s="37"/>
-      <c r="N34" s="37"/>
-    </row>
-    <row r="35" s="26" customFormat="1" ht="12" customHeight="1" spans="10:14">
-      <c r="J35" s="37"/>
-      <c r="N35" s="37"/>
+      <c r="J32" s="36"/>
+      <c r="N32" s="36"/>
+    </row>
+    <row r="33" s="26" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J33" s="36"/>
+      <c r="N33" s="36"/>
+    </row>
+    <row r="34" s="26" customFormat="1" ht="12" customHeight="1" spans="10:14">
+      <c r="J34" s="36"/>
+      <c r="N34" s="36"/>
+    </row>
+    <row r="35" s="26" customFormat="1" spans="10:14">
+      <c r="J35" s="36"/>
+      <c r="N35" s="36"/>
     </row>
     <row r="36" s="26" customFormat="1" spans="10:14">
-      <c r="J36" s="37"/>
-      <c r="N36" s="37"/>
-    </row>
-    <row r="37" s="26" customFormat="1" spans="10:14">
-      <c r="J37" s="37"/>
-      <c r="N37" s="37"/>
+      <c r="J36" s="36"/>
+      <c r="N36" s="36"/>
+    </row>
+    <row r="37" s="26" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J37" s="36"/>
+      <c r="N37" s="36"/>
     </row>
     <row r="38" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J38" s="37"/>
-      <c r="N38" s="37"/>
+      <c r="J38" s="36"/>
+      <c r="N38" s="36"/>
     </row>
     <row r="39" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J39" s="37"/>
-      <c r="N39" s="37"/>
+      <c r="J39" s="36"/>
+      <c r="N39" s="36"/>
     </row>
     <row r="40" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J40" s="37"/>
-      <c r="N40" s="37"/>
-    </row>
-    <row r="41" s="26" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J41" s="37"/>
-      <c r="N41" s="37"/>
+      <c r="J40" s="36"/>
+      <c r="N40" s="36"/>
+    </row>
+    <row r="41" s="26" customFormat="1" spans="10:14">
+      <c r="J41" s="36"/>
+      <c r="N41" s="36"/>
     </row>
     <row r="42" s="26" customFormat="1" spans="10:14">
-      <c r="J42" s="37"/>
-      <c r="N42" s="37"/>
+      <c r="J42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" s="26" customFormat="1" spans="10:14">
-      <c r="J43" s="37"/>
-      <c r="N43" s="37"/>
+      <c r="J43" s="36"/>
+      <c r="N43" s="36"/>
     </row>
     <row r="44" s="26" customFormat="1" spans="10:14">
-      <c r="J44" s="37"/>
-      <c r="N44" s="37"/>
+      <c r="J44" s="36"/>
+      <c r="N44" s="36"/>
     </row>
     <row r="45" s="26" customFormat="1" spans="10:14">
-      <c r="J45" s="37"/>
-      <c r="N45" s="37"/>
+      <c r="J45" s="36"/>
+      <c r="N45" s="36"/>
     </row>
     <row r="46" s="26" customFormat="1" spans="10:14">
-      <c r="J46" s="37"/>
-      <c r="N46" s="37"/>
+      <c r="J46" s="36"/>
+      <c r="N46" s="36"/>
     </row>
     <row r="47" s="26" customFormat="1" spans="10:14">
-      <c r="J47" s="37"/>
-      <c r="N47" s="37"/>
+      <c r="J47" s="36"/>
+      <c r="N47" s="36"/>
     </row>
     <row r="48" s="26" customFormat="1" spans="10:14">
-      <c r="J48" s="37"/>
-      <c r="N48" s="37"/>
+      <c r="J48" s="36"/>
+      <c r="N48" s="36"/>
     </row>
     <row r="49" s="26" customFormat="1" spans="10:14">
-      <c r="J49" s="37"/>
-      <c r="N49" s="37"/>
+      <c r="J49" s="36"/>
+      <c r="N49" s="36"/>
     </row>
     <row r="50" s="26" customFormat="1" spans="10:14">
-      <c r="J50" s="37"/>
-      <c r="N50" s="37"/>
+      <c r="J50" s="36"/>
+      <c r="N50" s="36"/>
     </row>
     <row r="51" s="26" customFormat="1" spans="10:14">
-      <c r="J51" s="37"/>
-      <c r="N51" s="37"/>
+      <c r="J51" s="36"/>
+      <c r="N51" s="36"/>
     </row>
     <row r="52" s="26" customFormat="1" spans="10:14">
-      <c r="J52" s="37"/>
-      <c r="N52" s="37"/>
+      <c r="J52" s="36"/>
+      <c r="N52" s="36"/>
     </row>
     <row r="53" s="26" customFormat="1" spans="10:14">
-      <c r="J53" s="37"/>
-      <c r="N53" s="37"/>
-    </row>
-    <row r="54" s="26" customFormat="1" spans="10:14">
-      <c r="J54" s="37"/>
-      <c r="N54" s="37"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="26"/>
+      <c r="J53" s="36"/>
+      <c r="N53" s="36"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="26"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the question text.&#10;&#10;It is advisable that you include the question number.&#10;&#10;E.g: 9. This is a question, what is the answer?" sqref="E40:E42"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="A5 C5 D5 A6:A10 A11:A1048576 B5:B10 B11:B1048576 C11:C1048576 D11:D12 D13:D1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the question text.&#10;&#10;It is advisable that you include the question number.&#10;&#10;E.g: 9. This is a question, what is the answer?" sqref="E39:E41"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="A5 B5 C5 D5 A6:A9 A10:A1048576 B6:B9 B10:B1048576 C10:C1048576 D10:D11 D12:D1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2054,16 +2018,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>17</v>
@@ -2071,212 +2035,212 @@
     </row>
     <row r="2" ht="12.75" customHeight="1" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" spans="1:4">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7">
         <v>0</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3679,7 +3643,7 @@
   <sheetPr/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3693,27 +3657,27 @@
   <sheetData>
     <row r="1" ht="15" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>

</xml_diff>